<commit_message>
turns out SR for CCEP is for KO oops
</commit_message>
<xml_diff>
--- a/data/company_info.xlsx
+++ b/data/company_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/Sustainable Finance Company wiki page with Langchain/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/Sustainable_Finance_Company_wiki_page_with_Langchain/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72995F2D-DAE9-4F4D-9639-83752846069D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B308DC15-C8C9-A544-B3A8-85CA73AC12EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9300" yWindow="660" windowWidth="19500" windowHeight="16260" xr2:uid="{4D933051-D078-B84E-9825-3D98AAA18220}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Symbol</t>
   </si>
@@ -140,15 +140,6 @@
     <t>Major Banks</t>
   </si>
   <si>
-    <t>CCEP</t>
-  </si>
-  <si>
-    <t>Coca-Cola Europacific Partners plc Ordinary Shares</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>Consumer Staples</t>
   </si>
   <si>
@@ -198,6 +189,15 @@
   </si>
   <si>
     <t>https://data.alibabagroup.com/ecms-files/1509739361/fcaefa3d-0989-48fb-b003-fa96aa04880e/2023%20Alibaba%20ESG%20Report-Final.pdf</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>Coca-Cola Company (The) Common Stock</t>
+  </si>
+  <si>
+    <t>2.53352E+11</t>
   </si>
 </sst>
 </file>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1F17EE-BBCB-0248-95E5-4DF4720A68F5}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,7 +653,7 @@
         <v>18</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>28</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -758,50 +758,50 @@
         <v>33</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1">
+        <v>58.6</v>
+      </c>
+      <c r="D6">
+        <v>-0.44</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <v>65172256</v>
+      </c>
+      <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="K6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="1">
-        <v>64.69</v>
-      </c>
-      <c r="D6">
-        <v>-0.24</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-3.7000000000000002E-3</v>
-      </c>
-      <c r="F6">
-        <v>29682760096</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6">
-        <v>30108857</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" t="s">
-        <v>38</v>
-      </c>
       <c r="M6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1">
         <v>114.12</v>
@@ -816,7 +816,7 @@
         <v>39893290617</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>2005</v>
@@ -828,18 +828,18 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1">
         <v>74.510000000000005</v>
@@ -851,10 +851,10 @@
         <v>2.76E-2</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H8">
         <v>2014</v>
@@ -866,10 +866,10 @@
         <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>